<commit_message>
discrete add lab3,4v7 and 4 done
</commit_message>
<xml_diff>
--- a/2 course/DiscreteMath/3/LABv20_exel.xlsx
+++ b/2 course/DiscreteMath/3/LABv20_exel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>t работы</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>R(5, конец)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Критический путь -R(начало),R(2),R(4),R(5),R(конец)  </t>
   </si>
 </sst>
 </file>
@@ -326,25 +329,25 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12114</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>13</xdr:col>
-          <xdr:colOff>2066925</xdr:colOff>
-          <xdr:row>13</xdr:row>
-          <xdr:rowOff>173630</xdr:rowOff>
+          <xdr:colOff>2562225</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>18876</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Object 1" hidden="1">
+            <xdr:cNvPr id="1027" name="Object 3" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
+                  <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -358,14 +361,28 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd type="none" w="med" len="med"/>
+            </a:ln>
+            <a:effectLst/>
             <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects>
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="808080"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
               </a:ext>
             </a:extLst>
           </xdr:spPr>
@@ -641,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X14"/>
+  <dimension ref="A1:X15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,8 +679,8 @@
     <col min="11" max="11" width="4.140625" customWidth="1"/>
     <col min="12" max="12" width="4.42578125" customWidth="1"/>
     <col min="13" max="13" width="4" customWidth="1"/>
-    <col min="14" max="14" width="32" customWidth="1"/>
-    <col min="15" max="15" width="43.42578125" customWidth="1"/>
+    <col min="14" max="14" width="39.140625" customWidth="1"/>
+    <col min="15" max="15" width="48.85546875" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" customWidth="1"/>
     <col min="17" max="17" width="11.42578125" customWidth="1"/>
     <col min="21" max="21" width="10.42578125" customWidth="1"/>
@@ -838,15 +855,15 @@
       </c>
       <c r="P3" s="7"/>
       <c r="Q3" s="12">
-        <f>S2-D2</f>
-        <v>9</v>
+        <f>S3-D2</f>
+        <v>12</v>
       </c>
       <c r="R3" s="12">
         <f>MIN(S3-E2,U3-F2)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="S3" s="12">
-        <f>MIN(V2-H2,T2-G2)</f>
+        <f>MIN(V2-H2,T3-G2)</f>
         <v>14</v>
       </c>
       <c r="T3" s="12">
@@ -854,11 +871,12 @@
         <v>23</v>
       </c>
       <c r="U3" s="12">
-        <f>MIN(V2-K2,V2-J2)</f>
-        <v>22</v>
+        <f>MIN(V2-K2,V2-J2,V2-(I2+L2))</f>
+        <v>19</v>
       </c>
       <c r="V3" s="7"/>
     </row>
+    <row r="4" spans="1:24" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O5" s="8" t="s">
         <v>35</v>
@@ -938,11 +956,11 @@
       </c>
       <c r="P7" s="9">
         <f>Q3</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="Q7" s="9">
         <f>R3</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="R7" s="9">
         <f>S3</f>
@@ -954,7 +972,7 @@
       </c>
       <c r="T7" s="9">
         <f>U3</f>
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="U7" s="9">
         <f>T3</f>
@@ -1009,11 +1027,11 @@
       </c>
       <c r="Q10" s="11">
         <f>Q3-Q2</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="R10" s="11">
         <f>R3-R2</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S10" s="11">
         <f>S3-S2</f>
@@ -1025,85 +1043,87 @@
       </c>
       <c r="U10" s="11">
         <f>U3-U2</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V10" s="11">
-        <f>V2</f>
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="O12" t="s">
+        <v>46</v>
+      </c>
       <c r="V12" s="1"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="O13" s="13" t="s">
+    <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O14" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P13" s="13" t="s">
+      <c r="P14" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="Q13" s="13" t="s">
+      <c r="Q14" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="R13" s="13" t="s">
+      <c r="R14" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="S13" s="13" t="s">
+      <c r="S14" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="T13" s="13" t="s">
+      <c r="T14" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="U13" s="13" t="s">
+      <c r="U14" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="V13" s="13" t="s">
+      <c r="V14" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="W13" s="13" t="s">
+      <c r="W14" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="X13" s="13" t="s">
+      <c r="X14" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="O14" s="13" t="s">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="O15" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="P14" s="6">
+      <c r="P15" s="6">
         <f>Q3-P2-B2</f>
-        <v>6</v>
-      </c>
-      <c r="Q14" s="6">
-        <f>R3-Q2-C2</f>
+        <v>9</v>
+      </c>
+      <c r="Q15" s="6">
+        <f>R3-P2-C2</f>
         <v>0</v>
       </c>
-      <c r="R14" s="6">
-        <f>S3-Q2-E2</f>
-        <v>5</v>
-      </c>
-      <c r="S14" s="6">
+      <c r="R15" s="6">
+        <f>S3-Q2-D2</f>
+        <v>9</v>
+      </c>
+      <c r="S15" s="6">
         <f>S3-R2-E2</f>
         <v>3</v>
       </c>
-      <c r="T14" s="6">
+      <c r="T15" s="6">
         <f>U3-R2-F2</f>
-        <v>3</v>
-      </c>
-      <c r="U14" s="6">
+        <v>0</v>
+      </c>
+      <c r="U15" s="6">
         <f>T3-S2-G2</f>
         <v>3</v>
       </c>
-      <c r="V14" s="6">
+      <c r="V15" s="6">
         <f>V2-S2-H2</f>
         <v>5</v>
       </c>
-      <c r="W14" s="6">
+      <c r="W15" s="6">
         <f>V2-T2-L2</f>
         <v>0</v>
       </c>
-      <c r="X14" s="6">
+      <c r="X15" s="6">
         <f>V2-U2-J3</f>
         <v>0</v>
       </c>
@@ -1132,9 +1152,9 @@
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Visio.Drawing.15" shapeId="1025" r:id="rId4">
+        <oleObject progId="Visio.Drawing.15" shapeId="1027" r:id="rId4">
           <objectPr defaultSize="0" autoPict="0" r:id="rId5">
-            <anchor moveWithCells="1" sizeWithCells="1">
+            <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
@@ -1143,16 +1163,16 @@
               </from>
               <to>
                 <xdr:col>13</xdr:col>
-                <xdr:colOff>2066925</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:colOff>2562225</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Visio.Drawing.15" shapeId="1025" r:id="rId4"/>
+        <oleObject progId="Visio.Drawing.15" shapeId="1027" r:id="rId4"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>

</xml_diff>